<commit_message>
Fix g i j endash emdash
</commit_message>
<xml_diff>
--- a/CMapLatin.xlsx
+++ b/CMapLatin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yueyu\Yueyu\Acy-Font\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B128338-9C2D-430C-8F2C-7B195951DFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4C1406-A6D2-4B6C-A2CB-3BDA38448349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{B974D762-1C9D-4D59-851B-F200FC16F2B9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>name (cid number)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -316,12 +316,6 @@
   </si>
   <si>
     <t>˝</t>
-  </si>
-  <si>
-    <t>–</t>
-  </si>
-  <si>
-    <t>—</t>
   </si>
   <si>
     <t>‚</t>
@@ -718,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49622BBA-CE7C-4AF1-84BA-B7F135521DA5}">
-  <dimension ref="A1:K102"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91:XFD92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
@@ -1788,14 +1782,14 @@
         <v>69</v>
       </c>
       <c r="B67">
-        <f t="shared" ref="B67:B102" si="2">_xlfn.UNICODE(A67)</f>
+        <f t="shared" ref="B67:B100" si="2">_xlfn.UNICODE(A67)</f>
         <v>245</v>
       </c>
       <c r="C67">
         <v>30349</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67:D102" si="3">"&lt;map code=""0x"&amp;DEC2HEX(B67)&amp;""" name=""cid"&amp;C67&amp;"""/&gt;"</f>
+        <f t="shared" ref="D67:D100" si="3">"&lt;map code=""0x"&amp;DEC2HEX(B67)&amp;""" name=""cid"&amp;C67&amp;"""/&gt;"</f>
         <v>&lt;map code="0xF5" name="cid30349"/&gt;</v>
       </c>
       <c r="K67" s="1"/>
@@ -2180,14 +2174,14 @@
       </c>
       <c r="B91">
         <f t="shared" si="2"/>
-        <v>8211</v>
+        <v>8218</v>
       </c>
       <c r="C91">
-        <v>30373</v>
+        <v>30375</v>
       </c>
       <c r="D91" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;map code="0x2013" name="cid30373"/&gt;</v>
+        <v>&lt;map code="0x201A" name="cid30375"/&gt;</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.5">
@@ -2196,14 +2190,14 @@
       </c>
       <c r="B92">
         <f t="shared" si="2"/>
-        <v>8212</v>
+        <v>8222</v>
       </c>
       <c r="C92">
-        <v>30374</v>
+        <v>30376</v>
       </c>
       <c r="D92" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;map code="0x2014" name="cid30374"/&gt;</v>
+        <v>&lt;map code="0x201E" name="cid30376"/&gt;</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.5">
@@ -2212,14 +2206,14 @@
       </c>
       <c r="B93">
         <f t="shared" si="2"/>
-        <v>8218</v>
+        <v>8224</v>
       </c>
       <c r="C93">
-        <v>30375</v>
+        <v>30377</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;map code="0x201A" name="cid30375"/&gt;</v>
+        <v>&lt;map code="0x2020" name="cid30377"/&gt;</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.5">
@@ -2228,14 +2222,14 @@
       </c>
       <c r="B94">
         <f t="shared" si="2"/>
-        <v>8222</v>
+        <v>8225</v>
       </c>
       <c r="C94">
-        <v>30376</v>
+        <v>30378</v>
       </c>
       <c r="D94" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;map code="0x201E" name="cid30376"/&gt;</v>
+        <v>&lt;map code="0x2021" name="cid30378"/&gt;</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.5">
@@ -2244,14 +2238,14 @@
       </c>
       <c r="B95">
         <f t="shared" si="2"/>
-        <v>8224</v>
+        <v>8249</v>
       </c>
       <c r="C95">
-        <v>30377</v>
+        <v>30379</v>
       </c>
       <c r="D95" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;map code="0x2020" name="cid30377"/&gt;</v>
+        <v>&lt;map code="0x2039" name="cid30379"/&gt;</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.5">
@@ -2260,14 +2254,14 @@
       </c>
       <c r="B96">
         <f t="shared" si="2"/>
-        <v>8225</v>
+        <v>8250</v>
       </c>
       <c r="C96">
-        <v>30378</v>
+        <v>30380</v>
       </c>
       <c r="D96" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;map code="0x2021" name="cid30378"/&gt;</v>
+        <v>&lt;map code="0x203A" name="cid30380"/&gt;</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.5">
@@ -2276,14 +2270,14 @@
       </c>
       <c r="B97">
         <f t="shared" si="2"/>
-        <v>8249</v>
+        <v>8260</v>
       </c>
       <c r="C97">
-        <v>30379</v>
+        <v>30381</v>
       </c>
       <c r="D97" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;map code="0x2039" name="cid30379"/&gt;</v>
+        <v>&lt;map code="0x2044" name="cid30381"/&gt;</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.5">
@@ -2292,14 +2286,14 @@
       </c>
       <c r="B98">
         <f t="shared" si="2"/>
-        <v>8250</v>
+        <v>8722</v>
       </c>
       <c r="C98">
-        <v>30380</v>
+        <v>30382</v>
       </c>
       <c r="D98" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;map code="0x203A" name="cid30380"/&gt;</v>
+        <v>&lt;map code="0x2212" name="cid30382"/&gt;</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.5">
@@ -2308,14 +2302,14 @@
       </c>
       <c r="B99">
         <f t="shared" si="2"/>
-        <v>8260</v>
+        <v>64257</v>
       </c>
       <c r="C99">
-        <v>30381</v>
+        <v>30383</v>
       </c>
       <c r="D99" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;map code="0x2044" name="cid30381"/&gt;</v>
+        <v>&lt;map code="0xFB01" name="cid30383"/&gt;</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.5">
@@ -2324,44 +2318,12 @@
       </c>
       <c r="B100">
         <f t="shared" si="2"/>
-        <v>8722</v>
+        <v>64258</v>
       </c>
       <c r="C100">
-        <v>30382</v>
+        <v>30384</v>
       </c>
       <c r="D100" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;map code="0x2212" name="cid30382"/&gt;</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A101" t="s">
-        <v>103</v>
-      </c>
-      <c r="B101">
-        <f t="shared" si="2"/>
-        <v>64257</v>
-      </c>
-      <c r="C101">
-        <v>30383</v>
-      </c>
-      <c r="D101" t="str">
-        <f t="shared" si="3"/>
-        <v>&lt;map code="0xFB01" name="cid30383"/&gt;</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A102" t="s">
-        <v>104</v>
-      </c>
-      <c r="B102">
-        <f t="shared" si="2"/>
-        <v>64258</v>
-      </c>
-      <c r="C102">
-        <v>30384</v>
-      </c>
-      <c r="D102" t="str">
         <f t="shared" si="3"/>
         <v>&lt;map code="0xFB02" name="cid30384"/&gt;</v>
       </c>

</xml_diff>